<commit_message>
Added speed of sound plot and spreadsheet
</commit_message>
<xml_diff>
--- a/PositioningSystemPractice/SpeedOfSoundProof.xlsx
+++ b/PositioningSystemPractice/SpeedOfSoundProof.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>speed of sound</t>
   </si>
@@ -24,10 +24,19 @@
     <t>inches/ms</t>
   </si>
   <si>
-    <t>actual distance</t>
+    <t>time (ms)</t>
   </si>
   <si>
-    <t>time</t>
+    <t>distance (m)</t>
+  </si>
+  <si>
+    <t>distance (in)</t>
+  </si>
+  <si>
+    <t>time (s)</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -93,6 +102,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Beacon Sonar</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Response Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -107,65 +140,116 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:trendline>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.30174809367103222"/>
+                  <c:y val="0.12539462559107731"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1400">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> y = 338.73x - 23.432
+R² = 0.9892</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:ln>
+              </c:spPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8400000000000011E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$D$6:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0.127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>0.48259999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>0.91439999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>1.6255999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89</c:v>
+                  <c:v>2.2605999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$6:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>78.400000000000006</c:v>
+                  <c:v>3.1749999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -180,50 +264,115 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95315648"/>
-        <c:axId val="95315072"/>
+        <c:axId val="93623360"/>
+        <c:axId val="93623936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95315648"/>
+        <c:axId val="93623360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Beacon Response Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95315072"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93623936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95315072"/>
+        <c:axId val="93623936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> (m)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95315648"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93623360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </a:solidFill>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -236,16 +385,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -554,20 +703,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,65 +727,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
       <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>5</v>
+      </c>
       <c r="D6">
-        <v>5</v>
+        <f>C6*0.0254</f>
+        <v>0.127</v>
       </c>
       <c r="E6">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f>E6/1000</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>19</v>
+      </c>
       <c r="D7">
-        <v>19</v>
+        <f t="shared" ref="D7:D11" si="0">C7*0.0254</f>
+        <v>0.48259999999999997</v>
       </c>
       <c r="E7">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" ref="F7:F11" si="1">E7/1000</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>36</v>
+      </c>
       <c r="D8">
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>0.91439999999999999</v>
       </c>
       <c r="E8">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>64</v>
+      </c>
       <c r="D9">
-        <v>64</v>
+        <f t="shared" si="0"/>
+        <v>1.6255999999999999</v>
       </c>
       <c r="E9">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>89</v>
+      </c>
       <c r="D10">
-        <v>89</v>
+        <f t="shared" si="0"/>
+        <v>2.2605999999999997</v>
       </c>
       <c r="E10">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>125</v>
+      </c>
       <c r="D11">
-        <v>125</v>
+        <f t="shared" si="0"/>
+        <v>3.1749999999999998</v>
       </c>
       <c r="E11">
         <v>78.400000000000006</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>7.8400000000000011E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>87.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>